<commit_message>
trying to figure out what's up
- I have no idea what's wrong
</commit_message>
<xml_diff>
--- a/New-Implementation/Data/complex-optimal.xlsx
+++ b/New-Implementation/Data/complex-optimal.xlsx
@@ -450,7 +450,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1219.003955250995</v>
+        <v>-29448.47694554488</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -479,7 +479,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>9.551792499119552</v>
+        <v>148.4419726943003</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>150.0000000000017</v>
       </c>
     </row>
     <row r="3">
@@ -534,7 +534,7 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>12.4057233321594</v>
+        <v>195.9914751892992</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>200.000000000005</v>
       </c>
     </row>
     <row r="4">
@@ -863,7 +863,7 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>9.551792499119554</v>
+        <v>148.9413865599024</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -887,7 +887,7 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>7.658275251635914</v>
+        <v>150.0000000000037</v>
       </c>
     </row>
     <row r="11">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>12.40572333215941</v>
+        <v>196.9711870599002</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>11.41572333215941</v>
+        <v>200.0000000000073</v>
       </c>
     </row>
     <row r="12">
@@ -1239,7 +1239,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>9.551792499119554</v>
+        <v>149.4458450099949</v>
       </c>
       <c r="J18" t="n">
         <v>1</v>
@@ -1263,7 +1263,7 @@
         </is>
       </c>
       <c r="O18" t="n">
-        <v>8.561792499119553</v>
+        <v>150.0000000000012</v>
       </c>
     </row>
     <row r="19">
@@ -1286,7 +1286,7 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>12.40572333215941</v>
+        <v>197.9607950099991</v>
       </c>
       <c r="J19" t="n">
         <v>1</v>
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="O19" t="n">
-        <v>11.4157233321594</v>
+        <v>200.0000000000016</v>
       </c>
     </row>
     <row r="20">
@@ -1615,7 +1615,7 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>9.551792499119554</v>
+        <v>149.9553990000011</v>
       </c>
       <c r="J26" t="n">
         <v>1</v>
@@ -1639,7 +1639,7 @@
         </is>
       </c>
       <c r="O26" t="n">
-        <v>7.658275251635914</v>
+        <v>149.9999999999973</v>
       </c>
     </row>
     <row r="27">
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>12.40572333215941</v>
+        <v>198.9603990000023</v>
       </c>
       <c r="J27" t="n">
         <v>1</v>
@@ -1686,7 +1686,7 @@
         </is>
       </c>
       <c r="O27" t="n">
-        <v>11.4157233321594</v>
+        <v>200.0000000000036</v>
       </c>
     </row>
     <row r="28">
@@ -1991,7 +1991,7 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>9.551792499119554</v>
+        <v>150.4700999999987</v>
       </c>
       <c r="J34" t="n">
         <v>1</v>
@@ -2015,7 +2015,7 @@
         </is>
       </c>
       <c r="O34" t="n">
-        <v>7.658275251635914</v>
+        <v>150.0000000000014</v>
       </c>
     </row>
     <row r="35">
@@ -2038,7 +2038,7 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>12.40572333215941</v>
+        <v>199.9701000000013</v>
       </c>
       <c r="J35" t="n">
         <v>1</v>
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="O35" t="n">
-        <v>11.41572333215941</v>
+        <v>200.0000000000041</v>
       </c>
     </row>
     <row r="36">
@@ -2367,7 +2367,7 @@
         </is>
       </c>
       <c r="I42" t="n">
-        <v>9.551792499119554</v>
+        <v>150.9900000000037</v>
       </c>
       <c r="J42" t="n">
         <v>1</v>
@@ -2391,7 +2391,7 @@
         </is>
       </c>
       <c r="O42" t="n">
-        <v>8.561792499119552</v>
+        <v>150.0000000000001</v>
       </c>
     </row>
     <row r="43">
@@ -2414,7 +2414,7 @@
         </is>
       </c>
       <c r="I43" t="n">
-        <v>12.40572333215941</v>
+        <v>200.9900000000083</v>
       </c>
       <c r="J43" t="n">
         <v>1</v>
@@ -2438,7 +2438,7 @@
         </is>
       </c>
       <c r="O43" t="n">
-        <v>11.4157233321594</v>
+        <v>200.0000000000048</v>
       </c>
     </row>
     <row r="44">
@@ -2743,7 +2743,7 @@
         </is>
       </c>
       <c r="I50" t="n">
-        <v>9.551792499119554</v>
+        <v>150.9900000000058</v>
       </c>
       <c r="J50" t="n">
         <v>1</v>
@@ -2767,7 +2767,7 @@
         </is>
       </c>
       <c r="O50" t="n">
-        <v>0</v>
+        <v>149.9999999999992</v>
       </c>
     </row>
     <row r="51">
@@ -2790,7 +2790,7 @@
         </is>
       </c>
       <c r="I51" t="n">
-        <v>12.40572333215941</v>
+        <v>200.9900000000049</v>
       </c>
       <c r="J51" t="n">
         <v>1</v>
@@ -2814,7 +2814,7 @@
         </is>
       </c>
       <c r="O51" t="n">
-        <v>0</v>
+        <v>200.000000000002</v>
       </c>
     </row>
     <row r="52">
@@ -2837,7 +2837,7 @@
         </is>
       </c>
       <c r="I52" t="n">
-        <v>9.967402422392594</v>
+        <v>307.1305050505151</v>
       </c>
       <c r="J52" t="n">
         <v>1</v>
@@ -2861,7 +2861,7 @@
         </is>
       </c>
       <c r="O52" t="n">
-        <v>76.58275251635914</v>
+        <v>406.1616161617819</v>
       </c>
     </row>
     <row r="53">
@@ -2884,7 +2884,7 @@
         </is>
       </c>
       <c r="I53" t="n">
-        <v>20.38749329725615</v>
+        <v>407.0805050505323</v>
       </c>
       <c r="J53" t="n">
         <v>1</v>
@@ -2908,7 +2908,7 @@
         </is>
       </c>
       <c r="O53" t="n">
-        <v>52.70516834423942</v>
+        <v>455.6060606060115</v>
       </c>
     </row>
     <row r="54">
@@ -3119,7 +3119,7 @@
         </is>
       </c>
       <c r="I58" t="n">
-        <v>9.551792499119554</v>
+        <v>150.9900000000043</v>
       </c>
       <c r="J58" t="n">
         <v>1</v>
@@ -3143,7 +3143,7 @@
         </is>
       </c>
       <c r="O58" t="n">
-        <v>0</v>
+        <v>150.000000000001</v>
       </c>
     </row>
     <row r="59">
@@ -3166,7 +3166,7 @@
         </is>
       </c>
       <c r="I59" t="n">
-        <v>12.40572333215941</v>
+        <v>200.990000000002</v>
       </c>
       <c r="J59" t="n">
         <v>1</v>
@@ -3190,7 +3190,7 @@
         </is>
       </c>
       <c r="O59" t="n">
-        <v>0</v>
+        <v>200.0000000000048</v>
       </c>
     </row>
     <row r="60">
@@ -3213,7 +3213,7 @@
         </is>
       </c>
       <c r="I60" t="n">
-        <v>9.967402422392624</v>
+        <v>0</v>
       </c>
       <c r="J60" t="n">
         <v>1</v>
@@ -3237,7 +3237,7 @@
         </is>
       </c>
       <c r="O60" t="n">
-        <v>76.58275251635908</v>
+        <v>406.1616161616134</v>
       </c>
     </row>
     <row r="61">
@@ -3260,7 +3260,7 @@
         </is>
       </c>
       <c r="I61" t="n">
-        <v>20.38749329725614</v>
+        <v>407.0805050505239</v>
       </c>
       <c r="J61" t="n">
         <v>1</v>
@@ -3284,7 +3284,7 @@
         </is>
       </c>
       <c r="O61" t="n">
-        <v>52.70516834423941</v>
+        <v>455.6060606060252</v>
       </c>
     </row>
     <row r="62">
@@ -3307,7 +3307,7 @@
         </is>
       </c>
       <c r="I62" t="n">
-        <v>0</v>
+        <v>307.130505050525</v>
       </c>
       <c r="J62" t="n">
         <v>1</v>
@@ -3495,7 +3495,7 @@
         </is>
       </c>
       <c r="I66" t="n">
-        <v>9.551792499119554</v>
+        <v>150.990000000002</v>
       </c>
       <c r="J66" t="n">
         <v>1</v>
@@ -3519,7 +3519,7 @@
         </is>
       </c>
       <c r="O66" t="n">
-        <v>0</v>
+        <v>150.0000000000001</v>
       </c>
     </row>
     <row r="67">
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="I67" t="n">
-        <v>12.40572333215941</v>
+        <v>200.9900000000014</v>
       </c>
       <c r="J67" t="n">
         <v>1</v>
@@ -3566,7 +3566,7 @@
         </is>
       </c>
       <c r="O67" t="n">
-        <v>0</v>
+        <v>200.0000000000006</v>
       </c>
     </row>
     <row r="68">
@@ -3589,7 +3589,7 @@
         </is>
       </c>
       <c r="I68" t="n">
-        <v>9.96740242239256</v>
+        <v>307.1305050505387</v>
       </c>
       <c r="J68" t="n">
         <v>1</v>
@@ -3613,7 +3613,7 @@
         </is>
       </c>
       <c r="O68" t="n">
-        <v>76.58275251635912</v>
+        <v>406.1616161616739</v>
       </c>
     </row>
     <row r="69">
@@ -3636,7 +3636,7 @@
         </is>
       </c>
       <c r="I69" t="n">
-        <v>0</v>
+        <v>407.0805050505073</v>
       </c>
       <c r="J69" t="n">
         <v>1</v>
@@ -3660,7 +3660,7 @@
         </is>
       </c>
       <c r="O69" t="n">
-        <v>52.70516834423943</v>
+        <v>455.6060606060639</v>
       </c>
     </row>
     <row r="70">
@@ -3730,7 +3730,7 @@
         </is>
       </c>
       <c r="I71" t="n">
-        <v>20.38749329725615</v>
+        <v>0</v>
       </c>
       <c r="J71" t="n">
         <v>1</v>
@@ -3871,7 +3871,7 @@
         </is>
       </c>
       <c r="I74" t="n">
-        <v>9.551792499119554</v>
+        <v>150.9900000000016</v>
       </c>
       <c r="J74" t="n">
         <v>1</v>
@@ -3895,7 +3895,7 @@
         </is>
       </c>
       <c r="O74" t="n">
-        <v>0</v>
+        <v>150.0000000000041</v>
       </c>
     </row>
     <row r="75">
@@ -3918,7 +3918,7 @@
         </is>
       </c>
       <c r="I75" t="n">
-        <v>12.40572333215941</v>
+        <v>200.9900000000019</v>
       </c>
       <c r="J75" t="n">
         <v>1</v>
@@ -3942,7 +3942,7 @@
         </is>
       </c>
       <c r="O75" t="n">
-        <v>0</v>
+        <v>200.0000000000029</v>
       </c>
     </row>
     <row r="76">
@@ -3965,7 +3965,7 @@
         </is>
       </c>
       <c r="I76" t="n">
-        <v>9.967402422392581</v>
+        <v>307.1305050505148</v>
       </c>
       <c r="J76" t="n">
         <v>1</v>
@@ -3989,7 +3989,7 @@
         </is>
       </c>
       <c r="O76" t="n">
-        <v>76.58275251635912</v>
+        <v>406.1616161616203</v>
       </c>
     </row>
     <row r="77">
@@ -4012,7 +4012,7 @@
         </is>
       </c>
       <c r="I77" t="n">
-        <v>20.38749329725615</v>
+        <v>407.0805050505035</v>
       </c>
       <c r="J77" t="n">
         <v>1</v>
@@ -4036,7 +4036,7 @@
         </is>
       </c>
       <c r="O77" t="n">
-        <v>52.70516834423943</v>
+        <v>455.6060606060926</v>
       </c>
     </row>
     <row r="78">
@@ -4247,7 +4247,7 @@
         </is>
       </c>
       <c r="I82" t="n">
-        <v>9.551792499119554</v>
+        <v>150.9900000000037</v>
       </c>
       <c r="J82" t="n">
         <v>1</v>
@@ -4271,7 +4271,7 @@
         </is>
       </c>
       <c r="O82" t="n">
-        <v>0</v>
+        <v>150.0000000000047</v>
       </c>
     </row>
     <row r="83">
@@ -4294,7 +4294,7 @@
         </is>
       </c>
       <c r="I83" t="n">
-        <v>12.40572333215941</v>
+        <v>200.990000000004</v>
       </c>
       <c r="J83" t="n">
         <v>1</v>
@@ -4318,7 +4318,7 @@
         </is>
       </c>
       <c r="O83" t="n">
-        <v>0</v>
+        <v>200.0000000000069</v>
       </c>
     </row>
     <row r="84">
@@ -4341,7 +4341,7 @@
         </is>
       </c>
       <c r="I84" t="n">
-        <v>9.967402422392592</v>
+        <v>307.1305050505004</v>
       </c>
       <c r="J84" t="n">
         <v>1</v>
@@ -4365,7 +4365,7 @@
         </is>
       </c>
       <c r="O84" t="n">
-        <v>76.58275251635909</v>
+        <v>406.1616161615236</v>
       </c>
     </row>
     <row r="85">
@@ -4388,7 +4388,7 @@
         </is>
       </c>
       <c r="I85" t="n">
-        <v>20.38749329725616</v>
+        <v>407.0805050505116</v>
       </c>
       <c r="J85" t="n">
         <v>1</v>
@@ -4412,7 +4412,7 @@
         </is>
       </c>
       <c r="O85" t="n">
-        <v>52.70516834423944</v>
+        <v>455.6060606059673</v>
       </c>
     </row>
     <row r="86">
@@ -4626,7 +4626,7 @@
         </is>
       </c>
       <c r="O90" t="n">
-        <v>0</v>
+        <v>148.4999999999957</v>
       </c>
     </row>
     <row r="91">
@@ -4652,7 +4652,7 @@
         </is>
       </c>
       <c r="O91" t="n">
-        <v>0</v>
+        <v>198.0000000000025</v>
       </c>
     </row>
     <row r="92">
@@ -4834,7 +4834,7 @@
         </is>
       </c>
       <c r="O98" t="n">
-        <v>7.571792499119556</v>
+        <v>148.4999999999999</v>
       </c>
     </row>
     <row r="99">
@@ -4860,7 +4860,7 @@
         </is>
       </c>
       <c r="O99" t="n">
-        <v>9.560933668847881</v>
+        <v>198.0000000000055</v>
       </c>
     </row>
     <row r="100">
@@ -5042,7 +5042,7 @@
         </is>
       </c>
       <c r="O106" t="n">
-        <v>7.571792499119553</v>
+        <v>148.5000000000005</v>
       </c>
     </row>
     <row r="107">
@@ -5068,7 +5068,7 @@
         </is>
       </c>
       <c r="O107" t="n">
-        <v>9.560933668847888</v>
+        <v>198.0000000000091</v>
       </c>
     </row>
     <row r="108">
@@ -5250,7 +5250,7 @@
         </is>
       </c>
       <c r="O114" t="n">
-        <v>6.678175251635913</v>
+        <v>148.5000000000006</v>
       </c>
     </row>
     <row r="115">
@@ -5276,7 +5276,7 @@
         </is>
       </c>
       <c r="O115" t="n">
-        <v>9.560933668847884</v>
+        <v>198.0000000000051</v>
       </c>
     </row>
     <row r="116">
@@ -5458,7 +5458,7 @@
         </is>
       </c>
       <c r="O122" t="n">
-        <v>7.571792499119554</v>
+        <v>148.4999999999986</v>
       </c>
     </row>
     <row r="123">
@@ -5484,7 +5484,7 @@
         </is>
       </c>
       <c r="O123" t="n">
-        <v>9.560933668847889</v>
+        <v>198.0000000000028</v>
       </c>
     </row>
     <row r="124">
@@ -5666,7 +5666,7 @@
         </is>
       </c>
       <c r="O130" t="n">
-        <v>7.571792499119552</v>
+        <v>159.0100000000062</v>
       </c>
     </row>
     <row r="131">
@@ -5692,7 +5692,7 @@
         </is>
       </c>
       <c r="O131" t="n">
-        <v>9.560933668847886</v>
+        <v>209.010000000003</v>
       </c>
     </row>
     <row r="132">
@@ -5874,7 +5874,7 @@
         </is>
       </c>
       <c r="O138" t="n">
-        <v>0</v>
+        <v>159.0100000000017</v>
       </c>
     </row>
     <row r="139">
@@ -5900,7 +5900,7 @@
         </is>
       </c>
       <c r="O139" t="n">
-        <v>0</v>
+        <v>209.0100000000014</v>
       </c>
     </row>
     <row r="140">
@@ -5926,7 +5926,7 @@
         </is>
       </c>
       <c r="O140" t="n">
-        <v>66.78175251635912</v>
+        <v>324.1816161616384</v>
       </c>
     </row>
     <row r="141">
@@ -5952,7 +5952,7 @@
         </is>
       </c>
       <c r="O141" t="n">
-        <v>47.80466834423944</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -6004,7 +6004,7 @@
         </is>
       </c>
       <c r="O143" t="n">
-        <v>0</v>
+        <v>423.6260606060823</v>
       </c>
     </row>
     <row r="144">
@@ -6082,7 +6082,7 @@
         </is>
       </c>
       <c r="O146" t="n">
-        <v>0</v>
+        <v>159.0100000000045</v>
       </c>
     </row>
     <row r="147">
@@ -6108,7 +6108,7 @@
         </is>
       </c>
       <c r="O147" t="n">
-        <v>0</v>
+        <v>209.0100000000044</v>
       </c>
     </row>
     <row r="148">
@@ -6134,7 +6134,7 @@
         </is>
       </c>
       <c r="O148" t="n">
-        <v>66.78175251635913</v>
+        <v>324.1816161615889</v>
       </c>
     </row>
     <row r="149">
@@ -6160,7 +6160,7 @@
         </is>
       </c>
       <c r="O149" t="n">
-        <v>47.80466834423944</v>
+        <v>423.6260606060694</v>
       </c>
     </row>
     <row r="150">
@@ -6290,7 +6290,7 @@
         </is>
       </c>
       <c r="O154" t="n">
-        <v>0</v>
+        <v>159.0100000000017</v>
       </c>
     </row>
     <row r="155">
@@ -6316,7 +6316,7 @@
         </is>
       </c>
       <c r="O155" t="n">
-        <v>0</v>
+        <v>209.0100000000048</v>
       </c>
     </row>
     <row r="156">
@@ -6342,7 +6342,7 @@
         </is>
       </c>
       <c r="O156" t="n">
-        <v>66.78175251635913</v>
+        <v>324.1816161616059</v>
       </c>
     </row>
     <row r="157">
@@ -6368,7 +6368,7 @@
         </is>
       </c>
       <c r="O157" t="n">
-        <v>47.80466834423944</v>
+        <v>423.626060606062</v>
       </c>
     </row>
     <row r="158">
@@ -6498,7 +6498,7 @@
         </is>
       </c>
       <c r="O162" t="n">
-        <v>0</v>
+        <v>159.009999999998</v>
       </c>
     </row>
     <row r="163">
@@ -6524,7 +6524,7 @@
         </is>
       </c>
       <c r="O163" t="n">
-        <v>0</v>
+        <v>209.0100000000014</v>
       </c>
     </row>
     <row r="164">
@@ -6550,7 +6550,7 @@
         </is>
       </c>
       <c r="O164" t="n">
-        <v>66.78175251635918</v>
+        <v>324.1816161616548</v>
       </c>
     </row>
     <row r="165">
@@ -6576,7 +6576,7 @@
         </is>
       </c>
       <c r="O165" t="n">
-        <v>0</v>
+        <v>423.6260606060977</v>
       </c>
     </row>
     <row r="166">
@@ -6628,7 +6628,7 @@
         </is>
       </c>
       <c r="O167" t="n">
-        <v>47.80466834423943</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -6706,7 +6706,7 @@
         </is>
       </c>
       <c r="O170" t="n">
-        <v>0</v>
+        <v>159.0100000000022</v>
       </c>
     </row>
     <row r="171">
@@ -6732,7 +6732,7 @@
         </is>
       </c>
       <c r="O171" t="n">
-        <v>0</v>
+        <v>209.0100000000064</v>
       </c>
     </row>
     <row r="172">
@@ -6758,7 +6758,7 @@
         </is>
       </c>
       <c r="O172" t="n">
-        <v>66.78175251635912</v>
+        <v>324.1816161616086</v>
       </c>
     </row>
     <row r="173">
@@ -6784,7 +6784,7 @@
         </is>
       </c>
       <c r="O173" t="n">
-        <v>47.80466834423942</v>
+        <v>423.6260606060716</v>
       </c>
     </row>
     <row r="174">
@@ -6914,7 +6914,7 @@
         </is>
       </c>
       <c r="O178" t="n">
-        <v>0</v>
+        <v>147.0150000000019</v>
       </c>
     </row>
     <row r="179">
@@ -6940,7 +6940,7 @@
         </is>
       </c>
       <c r="O179" t="n">
-        <v>0</v>
+        <v>196.0200000000053</v>
       </c>
     </row>
     <row r="180">
@@ -7122,7 +7122,7 @@
         </is>
       </c>
       <c r="O186" t="n">
-        <v>5.707876251635912</v>
+        <v>147.0149999999998</v>
       </c>
     </row>
     <row r="187">
@@ -7148,7 +7148,7 @@
         </is>
       </c>
       <c r="O187" t="n">
-        <v>8.590634668847882</v>
+        <v>196.0200000000048</v>
       </c>
     </row>
     <row r="188">
@@ -7330,7 +7330,7 @@
         </is>
       </c>
       <c r="O194" t="n">
-        <v>6.591692499119554</v>
+        <v>147.0149999999981</v>
       </c>
     </row>
     <row r="195">
@@ -7356,7 +7356,7 @@
         </is>
       </c>
       <c r="O195" t="n">
-        <v>9.445623332159403</v>
+        <v>196.020000000004</v>
       </c>
     </row>
     <row r="196">
@@ -7538,7 +7538,7 @@
         </is>
       </c>
       <c r="O202" t="n">
-        <v>6.591692499119554</v>
+        <v>147.0149999999956</v>
       </c>
     </row>
     <row r="203">
@@ -7564,7 +7564,7 @@
         </is>
       </c>
       <c r="O203" t="n">
-        <v>9.445623332159402</v>
+        <v>196.0200000000005</v>
       </c>
     </row>
     <row r="204">
@@ -7746,7 +7746,7 @@
         </is>
       </c>
       <c r="O210" t="n">
-        <v>6.591692499119552</v>
+        <v>157.4199000000034</v>
       </c>
     </row>
     <row r="211">
@@ -7772,7 +7772,7 @@
         </is>
       </c>
       <c r="O211" t="n">
-        <v>8.590634668847887</v>
+        <v>206.9199000000035</v>
       </c>
     </row>
     <row r="212">
@@ -7954,7 +7954,7 @@
         </is>
       </c>
       <c r="O218" t="n">
-        <v>5.707876251635914</v>
+        <v>158.029900000003</v>
       </c>
     </row>
     <row r="219">
@@ -7980,7 +7980,7 @@
         </is>
       </c>
       <c r="O219" t="n">
-        <v>8.590634668847876</v>
+        <v>208.0299000000039</v>
       </c>
     </row>
     <row r="220">
@@ -8162,7 +8162,7 @@
         </is>
       </c>
       <c r="O226" t="n">
-        <v>0</v>
+        <v>158.0299000000018</v>
       </c>
     </row>
     <row r="227">
@@ -8188,7 +8188,7 @@
         </is>
       </c>
       <c r="O227" t="n">
-        <v>0</v>
+        <v>208.0299000000021</v>
       </c>
     </row>
     <row r="228">
@@ -8214,7 +8214,7 @@
         </is>
       </c>
       <c r="O228" t="n">
-        <v>57.07876251635913</v>
+        <v>322.2214161616173</v>
       </c>
     </row>
     <row r="229">
@@ -8240,7 +8240,7 @@
         </is>
       </c>
       <c r="O229" t="n">
-        <v>42.95317334423943</v>
+        <v>421.6658606060573</v>
       </c>
     </row>
     <row r="230">
@@ -8370,7 +8370,7 @@
         </is>
       </c>
       <c r="O234" t="n">
-        <v>0</v>
+        <v>158.0298999999989</v>
       </c>
     </row>
     <row r="235">
@@ -8396,7 +8396,7 @@
         </is>
       </c>
       <c r="O235" t="n">
-        <v>0</v>
+        <v>208.0299000000009</v>
       </c>
     </row>
     <row r="236">
@@ -8422,7 +8422,7 @@
         </is>
       </c>
       <c r="O236" t="n">
-        <v>57.07876251635911</v>
+        <v>322.2214161615329</v>
       </c>
     </row>
     <row r="237">
@@ -8448,7 +8448,7 @@
         </is>
       </c>
       <c r="O237" t="n">
-        <v>42.95317334423942</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238">
@@ -8500,7 +8500,7 @@
         </is>
       </c>
       <c r="O239" t="n">
-        <v>0</v>
+        <v>421.6658606060817</v>
       </c>
     </row>
     <row r="240">
@@ -8578,7 +8578,7 @@
         </is>
       </c>
       <c r="O242" t="n">
-        <v>0</v>
+        <v>158.0299000000031</v>
       </c>
     </row>
     <row r="243">
@@ -8604,7 +8604,7 @@
         </is>
       </c>
       <c r="O243" t="n">
-        <v>0</v>
+        <v>208.0299000000059</v>
       </c>
     </row>
     <row r="244">
@@ -8630,7 +8630,7 @@
         </is>
       </c>
       <c r="O244" t="n">
-        <v>57.07876251635908</v>
+        <v>322.2214161616055</v>
       </c>
     </row>
     <row r="245">
@@ -8656,7 +8656,7 @@
         </is>
       </c>
       <c r="O245" t="n">
-        <v>42.95317334423943</v>
+        <v>421.6658606060504</v>
       </c>
     </row>
     <row r="246">
@@ -8786,7 +8786,7 @@
         </is>
       </c>
       <c r="O250" t="n">
-        <v>0</v>
+        <v>158.0299000000002</v>
       </c>
     </row>
     <row r="251">
@@ -8812,7 +8812,7 @@
         </is>
       </c>
       <c r="O251" t="n">
-        <v>0</v>
+        <v>208.0299000000083</v>
       </c>
     </row>
     <row r="252">
@@ -8838,7 +8838,7 @@
         </is>
       </c>
       <c r="O252" t="n">
-        <v>57.0787625163591</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253">
@@ -8864,7 +8864,7 @@
         </is>
       </c>
       <c r="O253" t="n">
-        <v>42.95317334423942</v>
+        <v>421.6658606060607</v>
       </c>
     </row>
     <row r="254">
@@ -8890,7 +8890,7 @@
         </is>
       </c>
       <c r="O254" t="n">
-        <v>0</v>
+        <v>322.2214161616082</v>
       </c>
     </row>
     <row r="255">
@@ -8994,7 +8994,7 @@
         </is>
       </c>
       <c r="O258" t="n">
-        <v>0</v>
+        <v>158.0299000000004</v>
       </c>
     </row>
     <row r="259">
@@ -9020,7 +9020,7 @@
         </is>
       </c>
       <c r="O259" t="n">
-        <v>0</v>
+        <v>208.0299000000055</v>
       </c>
     </row>
     <row r="260">
@@ -9046,7 +9046,7 @@
         </is>
       </c>
       <c r="O260" t="n">
-        <v>57.07876251635906</v>
+        <v>322.2214161616657</v>
       </c>
     </row>
     <row r="261">
@@ -9072,7 +9072,7 @@
         </is>
       </c>
       <c r="O261" t="n">
-        <v>42.95317334423944</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262">
@@ -9124,7 +9124,7 @@
         </is>
       </c>
       <c r="O263" t="n">
-        <v>0</v>
+        <v>421.6658606060753</v>
       </c>
     </row>
     <row r="264">
@@ -9202,7 +9202,7 @@
         </is>
       </c>
       <c r="O266" t="n">
-        <v>0</v>
+        <v>145.5448499999989</v>
       </c>
     </row>
     <row r="267">
@@ -9228,7 +9228,7 @@
         </is>
       </c>
       <c r="O267" t="n">
-        <v>0</v>
+        <v>194.0598000000099</v>
       </c>
     </row>
     <row r="268">
@@ -9410,7 +9410,7 @@
         </is>
       </c>
       <c r="O274" t="n">
-        <v>4.747280241635911</v>
+        <v>145.5448499999999</v>
       </c>
     </row>
     <row r="275">
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="O275" t="n">
-        <v>7.630038658847885</v>
+        <v>194.0598000000003</v>
       </c>
     </row>
     <row r="276">
@@ -9618,7 +9618,7 @@
         </is>
       </c>
       <c r="O282" t="n">
-        <v>4.747280241635915</v>
+        <v>145.5448499999953</v>
       </c>
     </row>
     <row r="283">
@@ -9644,7 +9644,7 @@
         </is>
       </c>
       <c r="O283" t="n">
-        <v>7.630038658847891</v>
+        <v>194.0597999999991</v>
       </c>
     </row>
     <row r="284">
@@ -9826,7 +9826,7 @@
         </is>
       </c>
       <c r="O290" t="n">
-        <v>4.747280241635917</v>
+        <v>155.8457010000022</v>
       </c>
     </row>
     <row r="291">
@@ -9852,7 +9852,7 @@
         </is>
       </c>
       <c r="O291" t="n">
-        <v>7.630038658847888</v>
+        <v>204.8507010000064</v>
       </c>
     </row>
     <row r="292">
@@ -10034,7 +10034,7 @@
         </is>
       </c>
       <c r="O298" t="n">
-        <v>4.747280241635915</v>
+        <v>156.4496010000029</v>
       </c>
     </row>
     <row r="299">
@@ -10060,7 +10060,7 @@
         </is>
       </c>
       <c r="O299" t="n">
-        <v>7.630038658847884</v>
+        <v>205.9496010000003</v>
       </c>
     </row>
     <row r="300">
@@ -10242,7 +10242,7 @@
         </is>
       </c>
       <c r="O306" t="n">
-        <v>5.621393499119554</v>
+        <v>157.0596010000013</v>
       </c>
     </row>
     <row r="307">
@@ -10268,7 +10268,7 @@
         </is>
       </c>
       <c r="O307" t="n">
-        <v>8.475324332159405</v>
+        <v>207.059601000002</v>
       </c>
     </row>
     <row r="308">
@@ -10450,7 +10450,7 @@
         </is>
       </c>
       <c r="O314" t="n">
-        <v>0</v>
+        <v>157.059601000001</v>
       </c>
     </row>
     <row r="315">
@@ -10476,7 +10476,7 @@
         </is>
       </c>
       <c r="O315" t="n">
-        <v>0</v>
+        <v>207.059601000001</v>
       </c>
     </row>
     <row r="316">
@@ -10502,7 +10502,7 @@
         </is>
       </c>
       <c r="O316" t="n">
-        <v>47.47280241635909</v>
+        <v>320.2808181616472</v>
       </c>
     </row>
     <row r="317">
@@ -10528,7 +10528,7 @@
         </is>
       </c>
       <c r="O317" t="n">
-        <v>38.15019329423942</v>
+        <v>419.7252626060918</v>
       </c>
     </row>
     <row r="318">
@@ -10658,7 +10658,7 @@
         </is>
       </c>
       <c r="O322" t="n">
-        <v>0</v>
+        <v>157.0596010000011</v>
       </c>
     </row>
     <row r="323">
@@ -10684,7 +10684,7 @@
         </is>
       </c>
       <c r="O323" t="n">
-        <v>0</v>
+        <v>207.059601000003</v>
       </c>
     </row>
     <row r="324">
@@ -10710,7 +10710,7 @@
         </is>
       </c>
       <c r="O324" t="n">
-        <v>47.47280241635916</v>
+        <v>0</v>
       </c>
     </row>
     <row r="325">
@@ -10736,7 +10736,7 @@
         </is>
       </c>
       <c r="O325" t="n">
-        <v>38.15019329423944</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326">
@@ -10762,7 +10762,7 @@
         </is>
       </c>
       <c r="O326" t="n">
-        <v>0</v>
+        <v>320.2808181615023</v>
       </c>
     </row>
     <row r="327">
@@ -10788,7 +10788,7 @@
         </is>
       </c>
       <c r="O327" t="n">
-        <v>0</v>
+        <v>419.725262606093</v>
       </c>
     </row>
     <row r="328">
@@ -10866,7 +10866,7 @@
         </is>
       </c>
       <c r="O330" t="n">
-        <v>0</v>
+        <v>157.0596009999985</v>
       </c>
     </row>
     <row r="331">
@@ -10892,7 +10892,7 @@
         </is>
       </c>
       <c r="O331" t="n">
-        <v>0</v>
+        <v>207.0596010000048</v>
       </c>
     </row>
     <row r="332">
@@ -10918,7 +10918,7 @@
         </is>
       </c>
       <c r="O332" t="n">
-        <v>47.47280241635914</v>
+        <v>320.2808181614398</v>
       </c>
     </row>
     <row r="333">
@@ -10944,7 +10944,7 @@
         </is>
       </c>
       <c r="O333" t="n">
-        <v>38.15019329423944</v>
+        <v>419.7252626060719</v>
       </c>
     </row>
     <row r="334">
@@ -11074,7 +11074,7 @@
         </is>
       </c>
       <c r="O338" t="n">
-        <v>0</v>
+        <v>157.0596010000052</v>
       </c>
     </row>
     <row r="339">
@@ -11100,7 +11100,7 @@
         </is>
       </c>
       <c r="O339" t="n">
-        <v>0</v>
+        <v>207.0596010000039</v>
       </c>
     </row>
     <row r="340">
@@ -11126,7 +11126,7 @@
         </is>
       </c>
       <c r="O340" t="n">
-        <v>47.47280241635916</v>
+        <v>320.2808181616836</v>
       </c>
     </row>
     <row r="341">
@@ -11152,7 +11152,7 @@
         </is>
       </c>
       <c r="O341" t="n">
-        <v>38.15019329423941</v>
+        <v>419.7252626060633</v>
       </c>
     </row>
     <row r="342">
@@ -11282,7 +11282,7 @@
         </is>
       </c>
       <c r="O346" t="n">
-        <v>0</v>
+        <v>157.0596010000041</v>
       </c>
     </row>
     <row r="347">
@@ -11308,7 +11308,7 @@
         </is>
       </c>
       <c r="O347" t="n">
-        <v>0</v>
+        <v>207.0596010000046</v>
       </c>
     </row>
     <row r="348">
@@ -11334,7 +11334,7 @@
         </is>
       </c>
       <c r="O348" t="n">
-        <v>47.47280241635916</v>
+        <v>320.2808181615999</v>
       </c>
     </row>
     <row r="349">
@@ -11360,7 +11360,7 @@
         </is>
       </c>
       <c r="O349" t="n">
-        <v>38.15019329423944</v>
+        <v>419.7252626060541</v>
       </c>
     </row>
     <row r="350">
@@ -11490,7 +11490,7 @@
         </is>
       </c>
       <c r="O354" t="n">
-        <v>0</v>
+        <v>144.0894015000007</v>
       </c>
     </row>
     <row r="355">
@@ -11516,7 +11516,7 @@
         </is>
       </c>
       <c r="O355" t="n">
-        <v>0</v>
+        <v>192.1192020000104</v>
       </c>
     </row>
     <row r="356">
@@ -11698,7 +11698,7 @@
         </is>
       </c>
       <c r="O362" t="n">
-        <v>4.660797489119553</v>
+        <v>144.0894014999973</v>
       </c>
     </row>
     <row r="363">
@@ -11724,7 +11724,7 @@
         </is>
       </c>
       <c r="O363" t="n">
-        <v>6.679048608947884</v>
+        <v>192.1192019999985</v>
       </c>
     </row>
     <row r="364">
@@ -11906,7 +11906,7 @@
         </is>
       </c>
       <c r="O370" t="n">
-        <v>3.796290191735913</v>
+        <v>154.2872439899992</v>
       </c>
     </row>
     <row r="371">
@@ -11932,7 +11932,7 @@
         </is>
       </c>
       <c r="O371" t="n">
-        <v>7.514728322159405</v>
+        <v>202.8021939900084</v>
       </c>
     </row>
     <row r="372">
@@ -12114,7 +12114,7 @@
         </is>
       </c>
       <c r="O378" t="n">
-        <v>4.660797489119552</v>
+        <v>154.8851049900048</v>
       </c>
     </row>
     <row r="379">
@@ -12140,7 +12140,7 @@
         </is>
       </c>
       <c r="O379" t="n">
-        <v>7.514728322159405</v>
+        <v>203.8901049900005</v>
       </c>
     </row>
     <row r="380">
@@ -12322,7 +12322,7 @@
         </is>
       </c>
       <c r="O386" t="n">
-        <v>4.660797489119559</v>
+        <v>155.4890049900015</v>
       </c>
     </row>
     <row r="387">
@@ -12348,7 +12348,7 @@
         </is>
       </c>
       <c r="O387" t="n">
-        <v>6.679048608947888</v>
+        <v>204.9890049899981</v>
       </c>
     </row>
     <row r="388">
@@ -12530,7 +12530,7 @@
         </is>
       </c>
       <c r="O394" t="n">
-        <v>4.660797489119554</v>
+        <v>156.0990049899995</v>
       </c>
     </row>
     <row r="395">
@@ -12556,7 +12556,7 @@
         </is>
       </c>
       <c r="O395" t="n">
-        <v>6.679048608947889</v>
+        <v>206.0990049900028</v>
       </c>
     </row>
     <row r="396">
@@ -12738,7 +12738,7 @@
         </is>
       </c>
       <c r="O402" t="n">
-        <v>0</v>
+        <v>156.0990049899972</v>
       </c>
     </row>
     <row r="403">
@@ -12764,7 +12764,7 @@
         </is>
       </c>
       <c r="O403" t="n">
-        <v>0</v>
+        <v>206.0990049900062</v>
       </c>
     </row>
     <row r="404">
@@ -12790,7 +12790,7 @@
         </is>
       </c>
       <c r="O404" t="n">
-        <v>37.96290191735915</v>
+        <v>318.3596261416708</v>
       </c>
     </row>
     <row r="405">
@@ -12816,7 +12816,7 @@
         </is>
       </c>
       <c r="O405" t="n">
-        <v>33.39524304473949</v>
+        <v>0</v>
       </c>
     </row>
     <row r="406">
@@ -12868,7 +12868,7 @@
         </is>
       </c>
       <c r="O407" t="n">
-        <v>0</v>
+        <v>417.8040705860635</v>
       </c>
     </row>
     <row r="408">
@@ -12946,7 +12946,7 @@
         </is>
       </c>
       <c r="O410" t="n">
-        <v>0</v>
+        <v>156.0990049900003</v>
       </c>
     </row>
     <row r="411">
@@ -12972,7 +12972,7 @@
         </is>
       </c>
       <c r="O411" t="n">
-        <v>0</v>
+        <v>206.0990049900044</v>
       </c>
     </row>
     <row r="412">
@@ -12998,7 +12998,7 @@
         </is>
       </c>
       <c r="O412" t="n">
-        <v>37.96290191735911</v>
+        <v>318.3596261416228</v>
       </c>
     </row>
     <row r="413">
@@ -13024,7 +13024,7 @@
         </is>
       </c>
       <c r="O413" t="n">
-        <v>33.39524304473942</v>
+        <v>417.804070586094</v>
       </c>
     </row>
     <row r="414">
@@ -13154,7 +13154,7 @@
         </is>
       </c>
       <c r="O418" t="n">
-        <v>0</v>
+        <v>156.0990049900087</v>
       </c>
     </row>
     <row r="419">
@@ -13180,7 +13180,7 @@
         </is>
       </c>
       <c r="O419" t="n">
-        <v>0</v>
+        <v>206.0990049900031</v>
       </c>
     </row>
     <row r="420">
@@ -13206,7 +13206,7 @@
         </is>
       </c>
       <c r="O420" t="n">
-        <v>37.96290191735915</v>
+        <v>318.359626141583</v>
       </c>
     </row>
     <row r="421">
@@ -13232,7 +13232,7 @@
         </is>
       </c>
       <c r="O421" t="n">
-        <v>33.39524304473942</v>
+        <v>417.8040705860524</v>
       </c>
     </row>
     <row r="422">
@@ -13362,7 +13362,7 @@
         </is>
       </c>
       <c r="O426" t="n">
-        <v>0</v>
+        <v>156.0990049899961</v>
       </c>
     </row>
     <row r="427">
@@ -13388,7 +13388,7 @@
         </is>
       </c>
       <c r="O427" t="n">
-        <v>0</v>
+        <v>206.0990049900043</v>
       </c>
     </row>
     <row r="428">
@@ -13414,7 +13414,7 @@
         </is>
       </c>
       <c r="O428" t="n">
-        <v>37.96290191735919</v>
+        <v>0</v>
       </c>
     </row>
     <row r="429">
@@ -13440,7 +13440,7 @@
         </is>
       </c>
       <c r="O429" t="n">
-        <v>33.39524304473943</v>
+        <v>417.8040705860968</v>
       </c>
     </row>
     <row r="430">
@@ -13466,7 +13466,7 @@
         </is>
       </c>
       <c r="O430" t="n">
-        <v>0</v>
+        <v>318.3596261416612</v>
       </c>
     </row>
     <row r="431">
@@ -13570,7 +13570,7 @@
         </is>
       </c>
       <c r="O434" t="n">
-        <v>0</v>
+        <v>156.0990049900059</v>
       </c>
     </row>
     <row r="435">
@@ -13596,7 +13596,7 @@
         </is>
       </c>
       <c r="O435" t="n">
-        <v>0</v>
+        <v>206.0990049900009</v>
       </c>
     </row>
     <row r="436">
@@ -13622,7 +13622,7 @@
         </is>
       </c>
       <c r="O436" t="n">
-        <v>37.96290191735918</v>
+        <v>318.3596261414818</v>
       </c>
     </row>
     <row r="437">
@@ -13648,7 +13648,7 @@
         </is>
       </c>
       <c r="O437" t="n">
-        <v>33.39524304473946</v>
+        <v>417.8040705860573</v>
       </c>
     </row>
     <row r="438">
@@ -13778,7 +13778,7 @@
         </is>
       </c>
       <c r="O442" t="n">
-        <v>0</v>
+        <v>142.6485074849967</v>
       </c>
     </row>
     <row r="443">
@@ -13804,7 +13804,7 @@
         </is>
       </c>
       <c r="O443" t="n">
-        <v>0</v>
+        <v>190.1980099799884</v>
       </c>
     </row>
     <row r="444">
@@ -13986,7 +13986,7 @@
         </is>
       </c>
       <c r="O450" t="n">
-        <v>2.854810042334905</v>
+        <v>152.7443715501</v>
       </c>
     </row>
     <row r="451">
@@ -14012,7 +14012,7 @@
         </is>
       </c>
       <c r="O451" t="n">
-        <v>5.737568459546885</v>
+        <v>200.7741720501126</v>
       </c>
     </row>
     <row r="452">
@@ -14194,7 +14194,7 @@
         </is>
       </c>
       <c r="O458" t="n">
-        <v>3.709807439219554</v>
+        <v>153.3362539401075</v>
       </c>
     </row>
     <row r="459">
@@ -14220,7 +14220,7 @@
         </is>
       </c>
       <c r="O459" t="n">
-        <v>5.737568459546887</v>
+        <v>201.8512039400995</v>
       </c>
     </row>
     <row r="460">
@@ -14402,7 +14402,7 @@
         </is>
       </c>
       <c r="O466" t="n">
-        <v>2.854810042334916</v>
+        <v>153.9341149401003</v>
       </c>
     </row>
     <row r="467">
@@ -14428,7 +14428,7 @@
         </is>
       </c>
       <c r="O467" t="n">
-        <v>5.737568459546888</v>
+        <v>202.9391149400993</v>
       </c>
     </row>
     <row r="468">
@@ -14610,7 +14610,7 @@
         </is>
       </c>
       <c r="O474" t="n">
-        <v>3.709807439219551</v>
+        <v>154.5380149401019</v>
       </c>
     </row>
     <row r="475">
@@ -14636,7 +14636,7 @@
         </is>
       </c>
       <c r="O475" t="n">
-        <v>5.737568459546892</v>
+        <v>204.0380149401005</v>
       </c>
     </row>
     <row r="476">
@@ -14818,7 +14818,7 @@
         </is>
       </c>
       <c r="O482" t="n">
-        <v>3.709807439219555</v>
+        <v>155.1480149401017</v>
       </c>
     </row>
     <row r="483">
@@ -14844,7 +14844,7 @@
         </is>
       </c>
       <c r="O483" t="n">
-        <v>5.737568459546887</v>
+        <v>205.148014940104</v>
       </c>
     </row>
     <row r="484">
@@ -15026,7 +15026,7 @@
         </is>
       </c>
       <c r="O490" t="n">
-        <v>0</v>
+        <v>155.1480149401005</v>
       </c>
     </row>
     <row r="491">
@@ -15052,7 +15052,7 @@
         </is>
       </c>
       <c r="O491" t="n">
-        <v>0</v>
+        <v>205.1480149401111</v>
       </c>
     </row>
     <row r="492">
@@ -15078,7 +15078,7 @@
         </is>
       </c>
       <c r="O492" t="n">
-        <v>0</v>
+        <v>316.45764604183</v>
       </c>
     </row>
     <row r="493">
@@ -15104,7 +15104,7 @@
         </is>
       </c>
       <c r="O493" t="n">
-        <v>28.68784229773444</v>
+        <v>415.9020904862476</v>
       </c>
     </row>
     <row r="494">
@@ -15130,7 +15130,7 @@
         </is>
       </c>
       <c r="O494" t="n">
-        <v>28.54810042334911</v>
+        <v>0</v>
       </c>
     </row>
     <row r="495">
@@ -15234,7 +15234,7 @@
         </is>
       </c>
       <c r="O498" t="n">
-        <v>0</v>
+        <v>155.1480149401043</v>
       </c>
     </row>
     <row r="499">
@@ -15260,7 +15260,7 @@
         </is>
       </c>
       <c r="O499" t="n">
-        <v>0</v>
+        <v>205.1480149401049</v>
       </c>
     </row>
     <row r="500">
@@ -15286,7 +15286,7 @@
         </is>
       </c>
       <c r="O500" t="n">
-        <v>28.54810042334913</v>
+        <v>316.45764604183</v>
       </c>
     </row>
     <row r="501">
@@ -15312,7 +15312,7 @@
         </is>
       </c>
       <c r="O501" t="n">
-        <v>28.68784229773443</v>
+        <v>415.9020904862456</v>
       </c>
     </row>
     <row r="502">
@@ -15442,7 +15442,7 @@
         </is>
       </c>
       <c r="O506" t="n">
-        <v>0</v>
+        <v>155.1480149401023</v>
       </c>
     </row>
     <row r="507">
@@ -15468,7 +15468,7 @@
         </is>
       </c>
       <c r="O507" t="n">
-        <v>0</v>
+        <v>205.1480149401105</v>
       </c>
     </row>
     <row r="508">
@@ -15494,7 +15494,7 @@
         </is>
       </c>
       <c r="O508" t="n">
-        <v>28.54810042334909</v>
+        <v>316.4576460417466</v>
       </c>
     </row>
     <row r="509">
@@ -15520,7 +15520,7 @@
         </is>
       </c>
       <c r="O509" t="n">
-        <v>28.68784229773442</v>
+        <v>415.90209048624</v>
       </c>
     </row>
     <row r="510">
@@ -15650,7 +15650,7 @@
         </is>
       </c>
       <c r="O514" t="n">
-        <v>0</v>
+        <v>155.1480149400991</v>
       </c>
     </row>
     <row r="515">
@@ -15676,7 +15676,7 @@
         </is>
       </c>
       <c r="O515" t="n">
-        <v>0</v>
+        <v>205.1480149401033</v>
       </c>
     </row>
     <row r="516">
@@ -15702,7 +15702,7 @@
         </is>
       </c>
       <c r="O516" t="n">
-        <v>28.54810042334914</v>
+        <v>316.4576460418921</v>
       </c>
     </row>
     <row r="517">
@@ -15728,7 +15728,7 @@
         </is>
       </c>
       <c r="O517" t="n">
-        <v>28.68784229773443</v>
+        <v>415.902090486283</v>
       </c>
     </row>
     <row r="518">
@@ -15858,7 +15858,7 @@
         </is>
       </c>
       <c r="O522" t="n">
-        <v>0</v>
+        <v>155.1480149401026</v>
       </c>
     </row>
     <row r="523">
@@ -15884,7 +15884,7 @@
         </is>
       </c>
       <c r="O523" t="n">
-        <v>0</v>
+        <v>205.1480149400991</v>
       </c>
     </row>
     <row r="524">
@@ -15910,7 +15910,7 @@
         </is>
       </c>
       <c r="O524" t="n">
-        <v>28.54810042334906</v>
+        <v>316.4576460418198</v>
       </c>
     </row>
     <row r="525">
@@ -15936,7 +15936,7 @@
         </is>
       </c>
       <c r="O525" t="n">
-        <v>28.68784229773441</v>
+        <v>415.9020904862802</v>
       </c>
     </row>
     <row r="526">
@@ -16066,7 +16066,7 @@
         </is>
       </c>
       <c r="O530" t="n">
-        <v>0</v>
+        <v>151.2169278345989</v>
       </c>
     </row>
     <row r="531">
@@ -16092,7 +16092,7 @@
         </is>
       </c>
       <c r="O531" t="n">
-        <v>0</v>
+        <v>198.7664303296119</v>
       </c>
     </row>
     <row r="532">
@@ -16274,7 +16274,7 @@
         </is>
       </c>
       <c r="O538" t="n">
-        <v>1.922744694427921</v>
+        <v>151.8028914007064</v>
       </c>
     </row>
     <row r="539">
@@ -16300,7 +16300,7 @@
         </is>
       </c>
       <c r="O539" t="n">
-        <v>4.805503111639879</v>
+        <v>199.8326919006978</v>
       </c>
     </row>
     <row r="540">
@@ -16482,7 +16482,7 @@
         </is>
       </c>
       <c r="O546" t="n">
-        <v>2.768327289818554</v>
+        <v>152.3947737906978</v>
       </c>
     </row>
     <row r="547">
@@ -16508,7 +16508,7 @@
         </is>
       </c>
       <c r="O547" t="n">
-        <v>4.805503111639897</v>
+        <v>200.9097237906983</v>
       </c>
     </row>
     <row r="548">
@@ -16690,7 +16690,7 @@
         </is>
       </c>
       <c r="O554" t="n">
-        <v>1.922744694427938</v>
+        <v>152.9926347907009</v>
       </c>
     </row>
     <row r="555">
@@ -16716,7 +16716,7 @@
         </is>
       </c>
       <c r="O555" t="n">
-        <v>5.622258122858405</v>
+        <v>201.9976347906968</v>
       </c>
     </row>
     <row r="556">
@@ -16898,7 +16898,7 @@
         </is>
       </c>
       <c r="O562" t="n">
-        <v>2.768327289818553</v>
+        <v>153.5965347907012</v>
       </c>
     </row>
     <row r="563">
@@ -16924,7 +16924,7 @@
         </is>
       </c>
       <c r="O563" t="n">
-        <v>4.805503111639895</v>
+        <v>203.0965347907008</v>
       </c>
     </row>
     <row r="564">
@@ -17106,7 +17106,7 @@
         </is>
       </c>
       <c r="O570" t="n">
-        <v>1.922744694427916</v>
+        <v>154.2065347907008</v>
       </c>
     </row>
     <row r="571">
@@ -17132,7 +17132,7 @@
         </is>
       </c>
       <c r="O571" t="n">
-        <v>4.805503111639895</v>
+        <v>204.2065347907003</v>
       </c>
     </row>
     <row r="572">
@@ -17314,7 +17314,7 @@
         </is>
       </c>
       <c r="O578" t="n">
-        <v>0</v>
+        <v>154.2065347907032</v>
       </c>
     </row>
     <row r="579">
@@ -17340,7 +17340,7 @@
         </is>
       </c>
       <c r="O579" t="n">
-        <v>0</v>
+        <v>204.206534790699</v>
       </c>
     </row>
     <row r="580">
@@ -17366,7 +17366,7 @@
         </is>
       </c>
       <c r="O580" t="n">
-        <v>19.22744694427924</v>
+        <v>314.5746857429497</v>
       </c>
     </row>
     <row r="581">
@@ -17392,7 +17392,7 @@
         </is>
       </c>
       <c r="O581" t="n">
-        <v>24.02751555819948</v>
+        <v>414.0191301874639</v>
       </c>
     </row>
     <row r="582">
@@ -17522,7 +17522,7 @@
         </is>
       </c>
       <c r="O586" t="n">
-        <v>0</v>
+        <v>154.2065347906959</v>
       </c>
     </row>
     <row r="587">
@@ -17548,7 +17548,7 @@
         </is>
       </c>
       <c r="O587" t="n">
-        <v>0</v>
+        <v>204.206534790702</v>
       </c>
     </row>
     <row r="588">
@@ -17574,7 +17574,7 @@
         </is>
       </c>
       <c r="O588" t="n">
-        <v>19.22744694427921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="589">
@@ -17600,7 +17600,7 @@
         </is>
       </c>
       <c r="O589" t="n">
-        <v>24.02751555819948</v>
+        <v>414.0191301874793</v>
       </c>
     </row>
     <row r="590">
@@ -17626,7 +17626,7 @@
         </is>
       </c>
       <c r="O590" t="n">
-        <v>0</v>
+        <v>314.5746857430393</v>
       </c>
     </row>
     <row r="591">
@@ -17730,7 +17730,7 @@
         </is>
       </c>
       <c r="O594" t="n">
-        <v>0</v>
+        <v>154.2065347907051</v>
       </c>
     </row>
     <row r="595">
@@ -17756,7 +17756,7 @@
         </is>
       </c>
       <c r="O595" t="n">
-        <v>0</v>
+        <v>204.2065347907032</v>
       </c>
     </row>
     <row r="596">
@@ -17782,7 +17782,7 @@
         </is>
       </c>
       <c r="O596" t="n">
-        <v>19.22744694427919</v>
+        <v>314.5746857429947</v>
       </c>
     </row>
     <row r="597">
@@ -17808,7 +17808,7 @@
         </is>
       </c>
       <c r="O597" t="n">
-        <v>24.02751555819948</v>
+        <v>414.0191301874694</v>
       </c>
     </row>
     <row r="598">
@@ -17938,7 +17938,7 @@
         </is>
       </c>
       <c r="O602" t="n">
-        <v>0</v>
+        <v>154.2065347907046</v>
       </c>
     </row>
     <row r="603">
@@ -17964,7 +17964,7 @@
         </is>
       </c>
       <c r="O603" t="n">
-        <v>0</v>
+        <v>204.2065347907038</v>
       </c>
     </row>
     <row r="604">
@@ -17990,7 +17990,7 @@
         </is>
       </c>
       <c r="O604" t="n">
-        <v>19.22744694427919</v>
+        <v>0</v>
       </c>
     </row>
     <row r="605">
@@ -18016,7 +18016,7 @@
         </is>
       </c>
       <c r="O605" t="n">
-        <v>0</v>
+        <v>414.019130187459</v>
       </c>
     </row>
     <row r="606">
@@ -18042,7 +18042,7 @@
         </is>
       </c>
       <c r="O606" t="n">
-        <v>0</v>
+        <v>314.5746857429431</v>
       </c>
     </row>
     <row r="607">
@@ -18068,7 +18068,7 @@
         </is>
       </c>
       <c r="O607" t="n">
-        <v>24.0275155581995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="608">
@@ -18146,7 +18146,7 @@
         </is>
       </c>
       <c r="O610" t="n">
-        <v>0</v>
+        <v>154.2065347907003</v>
       </c>
     </row>
     <row r="611">
@@ -18172,7 +18172,7 @@
         </is>
       </c>
       <c r="O611" t="n">
-        <v>0</v>
+        <v>204.2065347907049</v>
       </c>
     </row>
     <row r="612">
@@ -18198,7 +18198,7 @@
         </is>
       </c>
       <c r="O612" t="n">
-        <v>19.22744694427924</v>
+        <v>314.5746857430545</v>
       </c>
     </row>
     <row r="613">
@@ -18224,7 +18224,7 @@
         </is>
       </c>
       <c r="O613" t="n">
-        <v>24.02751555819949</v>
+        <v>414.0191301874615</v>
       </c>
     </row>
     <row r="614">
@@ -18354,7 +18354,7 @@
         </is>
       </c>
       <c r="O618" t="n">
-        <v>0</v>
+        <v>150.2848624866994</v>
       </c>
     </row>
     <row r="619">
@@ -18380,7 +18380,7 @@
         </is>
       </c>
       <c r="O619" t="n">
-        <v>0</v>
+        <v>197.8343649816908</v>
       </c>
     </row>
     <row r="620">
@@ -18562,7 +18562,7 @@
         </is>
       </c>
       <c r="O626" t="n">
-        <v>1</v>
+        <v>150.8708260527905</v>
       </c>
     </row>
     <row r="627">
@@ -18588,7 +18588,7 @@
         </is>
       </c>
       <c r="O627" t="n">
-        <v>3.882758417211972</v>
+        <v>198.9006265527874</v>
       </c>
     </row>
     <row r="628">
@@ -18770,7 +18770,7 @@
         </is>
       </c>
       <c r="O634" t="n">
-        <v>0.9999999999999973</v>
+        <v>151.4627084427931</v>
       </c>
     </row>
     <row r="635">
@@ -18796,7 +18796,7 @@
         </is>
       </c>
       <c r="O635" t="n">
-        <v>3.882758417211978</v>
+        <v>199.9776584427901</v>
       </c>
     </row>
     <row r="636">
@@ -18978,7 +18978,7 @@
         </is>
       </c>
       <c r="O642" t="n">
-        <v>1.000000000000004</v>
+        <v>152.0605694427903</v>
       </c>
     </row>
     <row r="643">
@@ -19004,7 +19004,7 @@
         </is>
       </c>
       <c r="O643" t="n">
-        <v>3.88275841721198</v>
+        <v>201.0655694427958</v>
       </c>
     </row>
     <row r="644">
@@ -19186,7 +19186,7 @@
         </is>
       </c>
       <c r="O650" t="n">
-        <v>1.000000000000002</v>
+        <v>152.6644694427941</v>
       </c>
     </row>
     <row r="651">
@@ -19212,7 +19212,7 @@
         </is>
       </c>
       <c r="O651" t="n">
-        <v>3.882758417211976</v>
+        <v>202.1644694427938</v>
       </c>
     </row>
     <row r="652">
@@ -19394,7 +19394,7 @@
         </is>
       </c>
       <c r="O658" t="n">
-        <v>1.83626194191155</v>
+        <v>153.2744694427881</v>
       </c>
     </row>
     <row r="659">
@@ -19420,7 +19420,7 @@
         </is>
       </c>
       <c r="O659" t="n">
-        <v>3.882758417211974</v>
+        <v>203.2744694427937</v>
       </c>
     </row>
     <row r="660">
@@ -19602,7 +19602,7 @@
         </is>
       </c>
       <c r="O666" t="n">
-        <v>1.836261941911563</v>
+        <v>153.2744694427919</v>
       </c>
     </row>
     <row r="667">
@@ -19628,7 +19628,7 @@
         </is>
       </c>
       <c r="O667" t="n">
-        <v>0</v>
+        <v>203.2744694427941</v>
       </c>
     </row>
     <row r="668">
@@ -19654,7 +19654,7 @@
         </is>
       </c>
       <c r="O668" t="n">
-        <v>0</v>
+        <v>312.7105550472529</v>
       </c>
     </row>
     <row r="669">
@@ -19680,7 +19680,7 @@
         </is>
       </c>
       <c r="O669" t="n">
-        <v>19.41379208605987</v>
+        <v>412.1549994916709</v>
       </c>
     </row>
     <row r="670">
@@ -19810,7 +19810,7 @@
         </is>
       </c>
       <c r="O674" t="n">
-        <v>0</v>
+        <v>153.2744694427943</v>
       </c>
     </row>
     <row r="675">
@@ -19836,7 +19836,7 @@
         </is>
       </c>
       <c r="O675" t="n">
-        <v>0</v>
+        <v>203.2744694427967</v>
       </c>
     </row>
     <row r="676">
@@ -19862,7 +19862,7 @@
         </is>
       </c>
       <c r="O676" t="n">
-        <v>9.999999999999943</v>
+        <v>312.710555047244</v>
       </c>
     </row>
     <row r="677">
@@ -19888,7 +19888,7 @@
         </is>
       </c>
       <c r="O677" t="n">
-        <v>19.41379208605987</v>
+        <v>412.1549994916646</v>
       </c>
     </row>
     <row r="678">
@@ -20018,7 +20018,7 @@
         </is>
       </c>
       <c r="O682" t="n">
-        <v>0</v>
+        <v>153.2744694427918</v>
       </c>
     </row>
     <row r="683">
@@ -20044,7 +20044,7 @@
         </is>
       </c>
       <c r="O683" t="n">
-        <v>0</v>
+        <v>203.2744694427957</v>
       </c>
     </row>
     <row r="684">
@@ -20070,7 +20070,7 @@
         </is>
       </c>
       <c r="O684" t="n">
-        <v>9.999999999999865</v>
+        <v>312.7105550472197</v>
       </c>
     </row>
     <row r="685">
@@ -20096,7 +20096,7 @@
         </is>
       </c>
       <c r="O685" t="n">
-        <v>19.41379208605984</v>
+        <v>412.1549994916728</v>
       </c>
     </row>
     <row r="686">
@@ -20226,7 +20226,7 @@
         </is>
       </c>
       <c r="O690" t="n">
-        <v>0</v>
+        <v>153.2744694427948</v>
       </c>
     </row>
     <row r="691">
@@ -20252,7 +20252,7 @@
         </is>
       </c>
       <c r="O691" t="n">
-        <v>0</v>
+        <v>203.2744694427976</v>
       </c>
     </row>
     <row r="692">
@@ -20278,7 +20278,7 @@
         </is>
       </c>
       <c r="O692" t="n">
-        <v>10.00000000000003</v>
+        <v>312.7105550472736</v>
       </c>
     </row>
     <row r="693">
@@ -20304,7 +20304,7 @@
         </is>
       </c>
       <c r="O693" t="n">
-        <v>0</v>
+        <v>412.1549994916253</v>
       </c>
     </row>
     <row r="694">
@@ -20356,7 +20356,7 @@
         </is>
       </c>
       <c r="O695" t="n">
-        <v>19.41379208605987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="696">
@@ -20434,7 +20434,7 @@
         </is>
       </c>
       <c r="O698" t="n">
-        <v>0</v>
+        <v>153.2744694427947</v>
       </c>
     </row>
     <row r="699">
@@ -20460,7 +20460,7 @@
         </is>
       </c>
       <c r="O699" t="n">
-        <v>0</v>
+        <v>203.2744694427982</v>
       </c>
     </row>
     <row r="700">
@@ -20486,7 +20486,7 @@
         </is>
       </c>
       <c r="O700" t="n">
-        <v>9.999999999999993</v>
+        <v>312.7105550472024</v>
       </c>
     </row>
     <row r="701">
@@ -20512,7 +20512,7 @@
         </is>
       </c>
       <c r="O701" t="n">
-        <v>19.41379208605987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="702">
@@ -20564,7 +20564,7 @@
         </is>
       </c>
       <c r="O703" t="n">
-        <v>0</v>
+        <v>412.1549994916256</v>
       </c>
     </row>
     <row r="704">
@@ -20642,7 +20642,7 @@
         </is>
       </c>
       <c r="O706" t="n">
-        <v>0</v>
+        <v>149.3621177922559</v>
       </c>
     </row>
     <row r="707">
@@ -20668,7 +20668,7 @@
         </is>
       </c>
       <c r="O707" t="n">
-        <v>0</v>
+        <v>196.9116202872619</v>
       </c>
     </row>
     <row r="708">
@@ -20850,7 +20850,7 @@
         </is>
       </c>
       <c r="O714" t="n">
-        <v>0.9135172474836413</v>
+        <v>149.9480813583636</v>
       </c>
     </row>
     <row r="715">
@@ -20876,7 +20876,7 @@
         </is>
       </c>
       <c r="O715" t="n">
-        <v>2.969241169728331</v>
+        <v>197.9778818583616</v>
       </c>
     </row>
     <row r="716">
@@ -21058,7 +21058,7 @@
         </is>
       </c>
       <c r="O722" t="n">
-        <v>0.9135172474836439</v>
+        <v>150.5399637483673</v>
       </c>
     </row>
     <row r="723">
@@ -21084,7 +21084,7 @@
         </is>
       </c>
       <c r="O723" t="n">
-        <v>3.767448080523494</v>
+        <v>199.0549137483701</v>
       </c>
     </row>
     <row r="724">
@@ -21266,7 +21266,7 @@
         </is>
       </c>
       <c r="O730" t="n">
-        <v>0.08648275251636006</v>
+        <v>151.1378247483661</v>
       </c>
     </row>
     <row r="731">
@@ -21292,7 +21292,7 @@
         </is>
       </c>
       <c r="O731" t="n">
-        <v>2.96924116972834</v>
+        <v>200.1428247483682</v>
       </c>
     </row>
     <row r="732">
@@ -21474,7 +21474,7 @@
         </is>
       </c>
       <c r="O738" t="n">
-        <v>0.9135172474836439</v>
+        <v>151.7417247483603</v>
       </c>
     </row>
     <row r="739">
@@ -21500,7 +21500,7 @@
         </is>
       </c>
       <c r="O739" t="n">
-        <v>3.767448080523486</v>
+        <v>201.241724748355</v>
       </c>
     </row>
     <row r="740">
@@ -21682,7 +21682,7 @@
         </is>
       </c>
       <c r="O746" t="n">
-        <v>0.9135172474836422</v>
+        <v>152.3517247483644</v>
       </c>
     </row>
     <row r="747">
@@ -21708,7 +21708,7 @@
         </is>
       </c>
       <c r="O747" t="n">
-        <v>2.969241169728338</v>
+        <v>202.3517247483708</v>
       </c>
     </row>
     <row r="748">
@@ -21890,7 +21890,7 @@
         </is>
       </c>
       <c r="O754" t="n">
-        <v>0</v>
+        <v>152.3517247483713</v>
       </c>
     </row>
     <row r="755">
@@ -21916,7 +21916,7 @@
         </is>
       </c>
       <c r="O755" t="n">
-        <v>0</v>
+        <v>202.3517247483718</v>
       </c>
     </row>
     <row r="756">
@@ -21942,7 +21942,7 @@
         </is>
       </c>
       <c r="O756" t="n">
-        <v>0.8648275251636157</v>
+        <v>310.8650656583361</v>
       </c>
     </row>
     <row r="757">
@@ -21968,7 +21968,7 @@
         </is>
       </c>
       <c r="O757" t="n">
-        <v>14.84620584864167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="758">
@@ -22020,7 +22020,7 @@
         </is>
       </c>
       <c r="O759" t="n">
-        <v>0</v>
+        <v>410.309510102781</v>
       </c>
     </row>
     <row r="760">
@@ -22098,7 +22098,7 @@
         </is>
       </c>
       <c r="O762" t="n">
-        <v>0</v>
+        <v>152.3517247483658</v>
       </c>
     </row>
     <row r="763">
@@ -22124,7 +22124,7 @@
         </is>
       </c>
       <c r="O763" t="n">
-        <v>0</v>
+        <v>202.3517247483734</v>
       </c>
     </row>
     <row r="764">
@@ -22150,7 +22150,7 @@
         </is>
       </c>
       <c r="O764" t="n">
-        <v>0.8648275251636264</v>
+        <v>310.8650656583643</v>
       </c>
     </row>
     <row r="765">
@@ -22176,7 +22176,7 @@
         </is>
       </c>
       <c r="O765" t="n">
-        <v>14.84620584864166</v>
+        <v>410.3095101027876</v>
       </c>
     </row>
     <row r="766">
@@ -22306,7 +22306,7 @@
         </is>
       </c>
       <c r="O770" t="n">
-        <v>0</v>
+        <v>152.3517247483745</v>
       </c>
     </row>
     <row r="771">
@@ -22332,7 +22332,7 @@
         </is>
       </c>
       <c r="O771" t="n">
-        <v>0</v>
+        <v>202.3517247483632</v>
       </c>
     </row>
     <row r="772">
@@ -22358,7 +22358,7 @@
         </is>
       </c>
       <c r="O772" t="n">
-        <v>0.8648275251636193</v>
+        <v>310.8650656582902</v>
       </c>
     </row>
     <row r="773">
@@ -22384,7 +22384,7 @@
         </is>
       </c>
       <c r="O773" t="n">
-        <v>14.84620584864167</v>
+        <v>410.3095101027816</v>
       </c>
     </row>
     <row r="774">
@@ -22514,7 +22514,7 @@
         </is>
       </c>
       <c r="O778" t="n">
-        <v>0</v>
+        <v>152.3517247483664</v>
       </c>
     </row>
     <row r="779">
@@ -22540,7 +22540,7 @@
         </is>
       </c>
       <c r="O779" t="n">
-        <v>0</v>
+        <v>202.3517247483585</v>
       </c>
     </row>
     <row r="780">
@@ -22566,7 +22566,7 @@
         </is>
       </c>
       <c r="O780" t="n">
-        <v>0.864827525163598</v>
+        <v>310.8650656583529</v>
       </c>
     </row>
     <row r="781">
@@ -22592,7 +22592,7 @@
         </is>
       </c>
       <c r="O781" t="n">
-        <v>14.84620584864169</v>
+        <v>410.309510102805</v>
       </c>
     </row>
     <row r="782">
@@ -22722,7 +22722,7 @@
         </is>
       </c>
       <c r="O786" t="n">
-        <v>0</v>
+        <v>152.3517247483602</v>
       </c>
     </row>
     <row r="787">
@@ -22748,7 +22748,7 @@
         </is>
       </c>
       <c r="O787" t="n">
-        <v>0</v>
+        <v>202.3517247483639</v>
       </c>
     </row>
     <row r="788">
@@ -22774,7 +22774,7 @@
         </is>
       </c>
       <c r="O788" t="n">
-        <v>0.8648275251636193</v>
+        <v>310.8650656584332</v>
       </c>
     </row>
     <row r="789">
@@ -22800,7 +22800,7 @@
         </is>
       </c>
       <c r="O789" t="n">
-        <v>14.84620584864166</v>
+        <v>410.309510102804</v>
       </c>
     </row>
     <row r="790">
@@ -22930,7 +22930,7 @@
         </is>
       </c>
       <c r="O794" t="n">
-        <v>0</v>
+        <v>148.44860054478</v>
       </c>
     </row>
     <row r="795">
@@ -22956,7 +22956,7 @@
         </is>
       </c>
       <c r="O795" t="n">
-        <v>0</v>
+        <v>195.998103039778</v>
       </c>
     </row>
     <row r="796">
@@ -23138,7 +23138,7 @@
         </is>
       </c>
       <c r="O802" t="n">
-        <v>0</v>
+        <v>149.0345641108852</v>
       </c>
     </row>
     <row r="803">
@@ -23164,7 +23164,7 @@
         </is>
       </c>
       <c r="O803" t="n">
-        <v>0</v>
+        <v>197.0643646108864</v>
       </c>
     </row>
     <row r="804">
@@ -23346,7 +23346,7 @@
         </is>
       </c>
       <c r="O810" t="n">
-        <v>0</v>
+        <v>149.6264465008829</v>
       </c>
     </row>
     <row r="811">
@@ -23372,7 +23372,7 @@
         </is>
       </c>
       <c r="O811" t="n">
-        <v>0</v>
+        <v>198.1413965008863</v>
       </c>
     </row>
     <row r="812">
@@ -23554,7 +23554,7 @@
         </is>
       </c>
       <c r="O818" t="n">
-        <v>0</v>
+        <v>150.2243075008766</v>
       </c>
     </row>
     <row r="819">
@@ -23580,7 +23580,7 @@
         </is>
       </c>
       <c r="O819" t="n">
-        <v>0</v>
+        <v>199.229307500874</v>
       </c>
     </row>
     <row r="820">
@@ -23762,7 +23762,7 @@
         </is>
       </c>
       <c r="O826" t="n">
-        <v>0</v>
+        <v>150.8282075008803</v>
       </c>
     </row>
     <row r="827">
@@ -23788,7 +23788,7 @@
         </is>
       </c>
       <c r="O827" t="n">
-        <v>0</v>
+        <v>200.32820750089</v>
       </c>
     </row>
     <row r="828">
@@ -23970,7 +23970,7 @@
         </is>
       </c>
       <c r="O834" t="n">
-        <v>0</v>
+        <v>151.438207500885</v>
       </c>
     </row>
     <row r="835">
@@ -23996,7 +23996,7 @@
         </is>
       </c>
       <c r="O835" t="n">
-        <v>0</v>
+        <v>201.4382075008828</v>
       </c>
     </row>
     <row r="836">
@@ -24178,7 +24178,7 @@
         </is>
       </c>
       <c r="O842" t="n">
-        <v>0</v>
+        <v>151.4382075008838</v>
       </c>
     </row>
     <row r="843">
@@ -24204,7 +24204,7 @@
         </is>
       </c>
       <c r="O843" t="n">
-        <v>0</v>
+        <v>201.4382075008879</v>
       </c>
     </row>
     <row r="844">
@@ -24386,7 +24386,7 @@
         </is>
       </c>
       <c r="O850" t="n">
-        <v>0</v>
+        <v>151.438207500883</v>
       </c>
     </row>
     <row r="851">
@@ -24412,7 +24412,7 @@
         </is>
       </c>
       <c r="O851" t="n">
-        <v>0</v>
+        <v>201.4382075008805</v>
       </c>
     </row>
     <row r="852">
@@ -24594,7 +24594,7 @@
         </is>
       </c>
       <c r="O858" t="n">
-        <v>0</v>
+        <v>151.4382075008832</v>
       </c>
     </row>
     <row r="859">
@@ -24620,7 +24620,7 @@
         </is>
       </c>
       <c r="O859" t="n">
-        <v>0</v>
+        <v>201.4382075008803</v>
       </c>
     </row>
     <row r="860">
@@ -24802,7 +24802,7 @@
         </is>
       </c>
       <c r="O866" t="n">
-        <v>0</v>
+        <v>151.438207500882</v>
       </c>
     </row>
     <row r="867">
@@ -24828,7 +24828,7 @@
         </is>
       </c>
       <c r="O867" t="n">
-        <v>0</v>
+        <v>201.4382075008841</v>
       </c>
     </row>
     <row r="868">
@@ -25010,7 +25010,7 @@
         </is>
       </c>
       <c r="O874" t="n">
-        <v>0</v>
+        <v>151.4382075008855</v>
       </c>
     </row>
     <row r="875">
@@ -25036,7 +25036,7 @@
         </is>
       </c>
       <c r="O875" t="n">
-        <v>0</v>
+        <v>201.4382075008838</v>
       </c>
     </row>
     <row r="876">

</xml_diff>